<commit_message>
Add golden chaas, masala chaas and improvised veg upma format
</commit_message>
<xml_diff>
--- a/Drinks/Golden chaas.xlsx
+++ b/Drinks/Golden chaas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandi\Google Drive\recipies\Drinks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E1A05B-5503-4A9A-8535-E0A2EFE41FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B277A92-47BD-4898-8C6F-A11161C82DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8CBC1288-2A94-44F0-92DE-D9C7067027C5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
   <si>
     <t>How many servings</t>
   </si>
@@ -111,9 +111,6 @@
     <t>black salt</t>
   </si>
   <si>
-    <t>gram</t>
-  </si>
-  <si>
     <t>water/curd ratio</t>
   </si>
   <si>
@@ -150,10 +147,10 @@
     <t>curry leaves paster</t>
   </si>
   <si>
-    <t xml:space="preserve"> springs</t>
-  </si>
-  <si>
     <t>rock salt</t>
+  </si>
+  <si>
+    <t>count</t>
   </si>
 </sst>
 </file>
@@ -223,7 +220,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -252,6 +249,9 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -755,7 +755,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +775,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -784,16 +784,16 @@
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -802,14 +802,14 @@
       </c>
       <c r="B2" s="7">
         <f>E2*F2/G2</f>
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2">
         <v>2.5</v>
@@ -818,7 +818,7 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="13">
         <f>F3/F2</f>
@@ -831,14 +831,14 @@
       </c>
       <c r="B3" s="7">
         <f t="shared" ref="B3:B11" si="0">E3*F3/G3</f>
-        <v>5.5</v>
+        <v>8.25</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
         <v>5.5</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="7">
         <f t="shared" si="0"/>
@@ -858,7 +858,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
@@ -867,21 +867,21 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0.75</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="G5" s="2">
         <v>2</v>
@@ -889,18 +889,18 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -911,18 +911,18 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="7">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1.125</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2">
         <v>0.75</v>
@@ -933,18 +933,18 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2">
         <v>0.5</v>
@@ -955,21 +955,21 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="B9" s="14">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G9" s="2">
         <v>2</v>
@@ -981,14 +981,14 @@
       </c>
       <c r="B10" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -999,18 +999,18 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="7">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>2.25</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="2">
         <v>1.5</v>

</xml_diff>